<commit_message>
REST-159 : Incorporated the review comments
</commit_message>
<xml_diff>
--- a/excel/src/test/resources/sample_data.xlsx
+++ b/excel/src/test/resources/sample_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lbade/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandar179178/Documents/GitHub/data-scalaxy-reader/excel/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4FE583-3807-FB44-B671-E88CF942E1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E93FB92-E067-6347-B2E6-C8123F6D25CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Zola</t>
   </si>
   <si>
-    <t>wlus9c76XX5j03st0cfuif174d6200000010498504</t>
-  </si>
-  <si>
     <t>CONFIRMED</t>
   </si>
   <si>
@@ -78,12 +75,6 @@
   </si>
   <si>
     <t>1210730000580100000</t>
-  </si>
-  <si>
-    <t>https://www.tradeinn.com/dressinn/es/bolsos-y-maletas/11074/lf#fq=id_familia=11074&amp;sort=precio_win_180;asc&amp;fe=&amp;pf=&amp;start=0</t>
-  </si>
-  <si>
-    <t>wles748eXX5j3jfuu8cuw38acf7500000085355591</t>
   </si>
   <si>
     <t>$12.48</t>
@@ -96,6 +87,15 @@
   </si>
   <si>
     <t>2022-04-18 07:23:54</t>
+  </si>
+  <si>
+    <t>wlus9</t>
+  </si>
+  <si>
+    <t>wles7</t>
+  </si>
+  <si>
+    <t>https://www.tradeinn.com/</t>
   </si>
 </sst>
 </file>
@@ -203,33 +203,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -460,10 +461,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1506,7 +1507,7 @@
   <dimension ref="A1:G951"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1521,15 +1522,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -1561,43 +1562,43 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>18</v>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>0.68</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2552,7 +2553,7 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" location="fq=id_familia=11074&amp;sort=precio_win_180;asc&amp;fe=&amp;pf=&amp;start=0" xr:uid="{4CE1DC10-EEDA-2245-9432-32A013B71A32}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{4CE1DC10-EEDA-2245-9432-32A013B71A32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>